<commit_message>
Update 21 May 2023
</commit_message>
<xml_diff>
--- a/IPL/Data/exp/gstats_fyaml.xlsx
+++ b/IPL/Data/exp/gstats_fyaml.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF122"/>
+  <dimension ref="A1:AF126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14115,6 +14115,454 @@
         <v>4</v>
       </c>
     </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2023-05-16</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Lucknow</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>1st innings</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>LSG</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>MI</t>
+        </is>
+      </c>
+      <c r="F123" t="n">
+        <v>1</v>
+      </c>
+      <c r="G123" t="n">
+        <v>167</v>
+      </c>
+      <c r="H123" t="n">
+        <v>34</v>
+      </c>
+      <c r="I123" t="n">
+        <v>77</v>
+      </c>
+      <c r="J123" t="n">
+        <v>56</v>
+      </c>
+      <c r="K123" t="n">
+        <v>4</v>
+      </c>
+      <c r="L123" t="n">
+        <v>2</v>
+      </c>
+      <c r="M123" t="n">
+        <v>2</v>
+      </c>
+      <c r="N123" t="n">
+        <v>0</v>
+      </c>
+      <c r="O123" t="n">
+        <v>125</v>
+      </c>
+      <c r="P123" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q123" t="n">
+        <v>63</v>
+      </c>
+      <c r="R123" t="n">
+        <v>26</v>
+      </c>
+      <c r="S123" t="inlineStr">
+        <is>
+          <t>2nd innings</t>
+        </is>
+      </c>
+      <c r="T123" t="inlineStr">
+        <is>
+          <t>LSG</t>
+        </is>
+      </c>
+      <c r="U123" t="n">
+        <v>157</v>
+      </c>
+      <c r="V123" t="n">
+        <v>55</v>
+      </c>
+      <c r="W123" t="n">
+        <v>71</v>
+      </c>
+      <c r="X123" t="n">
+        <v>31</v>
+      </c>
+      <c r="Y123" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z123" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA123" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB123" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC123" t="n">
+        <v>20</v>
+      </c>
+      <c r="AD123" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE123" t="n">
+        <v>10</v>
+      </c>
+      <c r="AF123" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2023-05-16</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Lucknow</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>2nd innings</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>MI</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>LSG</t>
+        </is>
+      </c>
+      <c r="F124" t="n">
+        <v>1</v>
+      </c>
+      <c r="G124" t="n">
+        <v>157</v>
+      </c>
+      <c r="H124" t="n">
+        <v>55</v>
+      </c>
+      <c r="I124" t="n">
+        <v>71</v>
+      </c>
+      <c r="J124" t="n">
+        <v>31</v>
+      </c>
+      <c r="K124" t="n">
+        <v>5</v>
+      </c>
+      <c r="L124" t="n">
+        <v>0</v>
+      </c>
+      <c r="M124" t="n">
+        <v>3</v>
+      </c>
+      <c r="N124" t="n">
+        <v>2</v>
+      </c>
+      <c r="O124" t="n">
+        <v>130</v>
+      </c>
+      <c r="P124" t="n">
+        <v>39</v>
+      </c>
+      <c r="Q124" t="n">
+        <v>62</v>
+      </c>
+      <c r="R124" t="n">
+        <v>29</v>
+      </c>
+      <c r="S124" t="inlineStr">
+        <is>
+          <t>1st innings</t>
+        </is>
+      </c>
+      <c r="T124" t="inlineStr">
+        <is>
+          <t>MI</t>
+        </is>
+      </c>
+      <c r="U124" t="n">
+        <v>167</v>
+      </c>
+      <c r="V124" t="n">
+        <v>34</v>
+      </c>
+      <c r="W124" t="n">
+        <v>77</v>
+      </c>
+      <c r="X124" t="n">
+        <v>56</v>
+      </c>
+      <c r="Y124" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z124" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA124" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB124" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC124" t="n">
+        <v>20</v>
+      </c>
+      <c r="AD124" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE124" t="n">
+        <v>10</v>
+      </c>
+      <c r="AF124" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2023-05-17</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Dharamsala</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>1st innings</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>PBKS</t>
+        </is>
+      </c>
+      <c r="F125" t="n">
+        <v>1</v>
+      </c>
+      <c r="G125" t="n">
+        <v>208</v>
+      </c>
+      <c r="H125" t="n">
+        <v>60</v>
+      </c>
+      <c r="I125" t="n">
+        <v>91</v>
+      </c>
+      <c r="J125" t="n">
+        <v>57</v>
+      </c>
+      <c r="K125" t="n">
+        <v>2</v>
+      </c>
+      <c r="L125" t="n">
+        <v>0</v>
+      </c>
+      <c r="M125" t="n">
+        <v>2</v>
+      </c>
+      <c r="N125" t="n">
+        <v>0</v>
+      </c>
+      <c r="O125" t="n">
+        <v>125</v>
+      </c>
+      <c r="P125" t="n">
+        <v>37</v>
+      </c>
+      <c r="Q125" t="n">
+        <v>62</v>
+      </c>
+      <c r="R125" t="n">
+        <v>26</v>
+      </c>
+      <c r="S125" t="inlineStr">
+        <is>
+          <t>2nd innings</t>
+        </is>
+      </c>
+      <c r="T125" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
+      <c r="U125" t="n">
+        <v>188</v>
+      </c>
+      <c r="V125" t="n">
+        <v>44</v>
+      </c>
+      <c r="W125" t="n">
+        <v>87</v>
+      </c>
+      <c r="X125" t="n">
+        <v>57</v>
+      </c>
+      <c r="Y125" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z125" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA125" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB125" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC125" t="n">
+        <v>20</v>
+      </c>
+      <c r="AD125" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE125" t="n">
+        <v>10</v>
+      </c>
+      <c r="AF125" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2023-05-17</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Dharamsala</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>2nd innings</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>PBKS</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
+      <c r="F126" t="n">
+        <v>1</v>
+      </c>
+      <c r="G126" t="n">
+        <v>188</v>
+      </c>
+      <c r="H126" t="n">
+        <v>44</v>
+      </c>
+      <c r="I126" t="n">
+        <v>87</v>
+      </c>
+      <c r="J126" t="n">
+        <v>57</v>
+      </c>
+      <c r="K126" t="n">
+        <v>8</v>
+      </c>
+      <c r="L126" t="n">
+        <v>1</v>
+      </c>
+      <c r="M126" t="n">
+        <v>3</v>
+      </c>
+      <c r="N126" t="n">
+        <v>4</v>
+      </c>
+      <c r="O126" t="n">
+        <v>124</v>
+      </c>
+      <c r="P126" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q126" t="n">
+        <v>61</v>
+      </c>
+      <c r="R126" t="n">
+        <v>27</v>
+      </c>
+      <c r="S126" t="inlineStr">
+        <is>
+          <t>1st innings</t>
+        </is>
+      </c>
+      <c r="T126" t="inlineStr">
+        <is>
+          <t>PBKS</t>
+        </is>
+      </c>
+      <c r="U126" t="n">
+        <v>208</v>
+      </c>
+      <c r="V126" t="n">
+        <v>60</v>
+      </c>
+      <c r="W126" t="n">
+        <v>91</v>
+      </c>
+      <c r="X126" t="n">
+        <v>57</v>
+      </c>
+      <c r="Y126" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z126" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA126" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB126" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC126" t="n">
+        <v>20</v>
+      </c>
+      <c r="AD126" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE126" t="n">
+        <v>10</v>
+      </c>
+      <c r="AF126" t="n">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>